<commit_message>
Add detail comment into template_sqlcreate.xlsx
</commit_message>
<xml_diff>
--- a/template_data/template_sqlcreate.xlsx
+++ b/template_data/template_sqlcreate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\study\python\xlsqlcreate\template_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2094C518-A6C6-4A94-B9A9-D46B433731C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F0540D-0C76-4679-9E61-D0654B8443DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7515" yWindow="4455" windowWidth="18075" windowHeight="12945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="2580" windowWidth="14970" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="2" r:id="rId1"/>
@@ -502,6 +502,84 @@
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>INSERT INTO user_tbl(id, name, birth) VALUES (8, '', '');</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="吹き出し: 四角形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6447F22-6E01-49BF-BB91-6F849F7DB180}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10267950" y="190500"/>
+          <a:ext cx="2609850" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -58833"/>
+            <a:gd name="adj2" fmla="val -23055"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Entering the title item is not mandatory.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>It is</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> to make it easier to understand.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -775,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B4A1E0-1742-40DB-AD19-879B6222DF77}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -902,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>

</xml_diff>